<commit_message>
moving to work pc
</commit_message>
<xml_diff>
--- a/LOGS.xlsx
+++ b/LOGS.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0E8E81-7F09-4369-8E13-DC46E7DABB9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Errors" sheetId="1" r:id="rId1"/>
     <sheet name="Estimates" sheetId="2" r:id="rId2"/>
     <sheet name="Regex And Code Conventions" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -168,9 +169,6 @@
     <t>match text between 2 strings</t>
   </si>
   <si>
-    <t>(?&lt;=&lt;str1&gt;)(.*)(?=&lt;str2&gt;)</t>
-  </si>
-  <si>
     <t>^((?!&lt;str&gt;).)*$</t>
   </si>
   <si>
@@ -181,12 +179,15 @@
   </si>
   <si>
     <t>match everything outside square paranthesis</t>
+  </si>
+  <si>
+    <t>(?&lt;=str1)(.*)(?=str2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -382,6 +383,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -417,6 +435,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -592,23 +627,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.44140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="76" style="5" customWidth="1"/>
-    <col min="4" max="4" width="27.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>15</v>
       </c>
@@ -619,7 +654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
@@ -637,7 +672,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
@@ -648,7 +683,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
@@ -659,7 +694,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -670,7 +705,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -681,7 +716,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
@@ -692,7 +727,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
@@ -703,7 +738,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -714,7 +749,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
@@ -725,7 +760,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
@@ -736,7 +771,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
@@ -747,7 +782,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>32</v>
       </c>
@@ -758,7 +793,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
@@ -776,25 +811,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="3"/>
-    <col min="2" max="2" width="41.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="3"/>
-    <col min="6" max="6" width="11.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="41.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="3"/>
+    <col min="6" max="6" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>22</v>
       </c>
@@ -817,7 +852,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>43633</v>
       </c>
@@ -842,23 +877,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="39.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="51.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="56" style="1" customWidth="1"/>
-    <col min="4" max="4" width="55.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="1"/>
+    <col min="4" max="4" width="55.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>39</v>
       </c>
@@ -872,7 +907,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>36</v>
       </c>
@@ -886,17 +921,17 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>46</v>
       </c>
@@ -907,28 +942,28 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="1" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>